<commit_message>
Revert "Subindo dados atualizados"
This reverts commit 4869b6ebd65744c064eb37899b19058b2120108c.
</commit_message>
<xml_diff>
--- a/Dados/DadosGerminacao.xlsx
+++ b/Dados/DadosGerminacao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Biblioteca\Documentos\USP\FCD\Projeto-Sementes\Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Biblioteca\Documentos\USP\FCD\Projeto-Sementes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0222732D-11DD-4768-8C86-E4DF8089EE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD3CFDA-C944-4977-9DB6-F00D25A184F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{5824C614-D8C0-4EF2-AFFD-50FAD2E80C64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5824C614-D8C0-4EF2-AFFD-50FAD2E80C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>0 Dias</t>
+  </si>
+  <si>
+    <t>5 Dias</t>
+  </si>
+  <si>
+    <t>10 Dias</t>
+  </si>
+  <si>
+    <t>15 Dias</t>
+  </si>
   <si>
     <t>Controle</t>
   </si>
@@ -207,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -225,9 +237,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +554,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,22 +565,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="11">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5">
-        <v>15</v>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
@@ -589,7 +598,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -606,7 +615,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -623,7 +632,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" s="9">
         <v>3</v>

</xml_diff>